<commit_message>
Updated schematic(actually have a pdf this time, you're welcome Joss....) and pin mappings in the spread sheet. 8 LED pins, 12 GPIO, and a buzzer
</commit_message>
<xml_diff>
--- a/FreescalePinMap.xlsx
+++ b/FreescalePinMap.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>Radio</t>
   </si>
@@ -110,97 +111,190 @@
     <t>J1 9</t>
   </si>
   <si>
-    <t>J1 5</t>
-  </si>
-  <si>
     <t>J1 1</t>
   </si>
   <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Odd pins on top -  higher numbers are farther to the right when looking at the back</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>LED5</t>
+  </si>
+  <si>
+    <t>LED6</t>
+  </si>
+  <si>
+    <t>LED7</t>
+  </si>
+  <si>
+    <t>LED8</t>
+  </si>
+  <si>
+    <t>LED_BANK_1</t>
+  </si>
+  <si>
+    <t>LED_BANK_2</t>
+  </si>
+  <si>
+    <t>GPIO_BANK_1</t>
+  </si>
+  <si>
+    <t>GPIO_BANK_2</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
+  </si>
+  <si>
+    <t>GPIO6</t>
+  </si>
+  <si>
+    <t>GPIO7</t>
+  </si>
+  <si>
+    <t>GPIO8</t>
+  </si>
+  <si>
+    <t>GPIO9</t>
+  </si>
+  <si>
+    <t>GPIO10</t>
+  </si>
+  <si>
+    <t>GPIO11</t>
+  </si>
+  <si>
+    <t>PTC6</t>
+  </si>
+  <si>
+    <t>PTC5</t>
+  </si>
+  <si>
+    <t>J1 3</t>
+  </si>
+  <si>
+    <t>PTC7</t>
+  </si>
+  <si>
+    <t>PTC0</t>
+  </si>
+  <si>
+    <t>PTE30</t>
+  </si>
+  <si>
+    <t>J10 11</t>
+  </si>
+  <si>
+    <t>200 ohm resistor and mosfet on ground side of all leds</t>
+  </si>
+  <si>
+    <t>J1 14</t>
+  </si>
+  <si>
+    <t>J1 16</t>
+  </si>
+  <si>
+    <t>J1 15</t>
+  </si>
+  <si>
+    <t>J1 13</t>
+  </si>
+  <si>
+    <t>J2 1</t>
+  </si>
+  <si>
+    <t>J2 5</t>
+  </si>
+  <si>
     <t>J1 6</t>
   </si>
   <si>
     <t>J1 8</t>
   </si>
   <si>
+    <t>J2 9</t>
+  </si>
+  <si>
+    <t>J1 10</t>
+  </si>
+  <si>
     <t>J1 12</t>
   </si>
   <si>
-    <t>J1 14</t>
-  </si>
-  <si>
-    <t>J1 16</t>
-  </si>
-  <si>
-    <t>J1 10</t>
-  </si>
-  <si>
-    <t>GPIO2</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
-    <t>J2 1</t>
-  </si>
-  <si>
-    <t>J9 10</t>
-  </si>
-  <si>
-    <t>J1 15</t>
-  </si>
-  <si>
-    <t>J1 13</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>GND   -top left</t>
-  </si>
-  <si>
-    <t>5V   -lower left</t>
-  </si>
-  <si>
-    <t>1 PTC12</t>
-  </si>
-  <si>
-    <t>1 PTC8</t>
-  </si>
-  <si>
-    <t>1 PTC9</t>
-  </si>
-  <si>
-    <t>1 PTC10</t>
-  </si>
-  <si>
-    <t>1 PTC11</t>
-  </si>
-  <si>
-    <t>1 PTC6</t>
-  </si>
-  <si>
-    <t>1 PTC7</t>
-  </si>
-  <si>
-    <t>1 PTC5</t>
-  </si>
-  <si>
-    <t>1 PTC3</t>
-  </si>
-  <si>
-    <t>1 PTD4</t>
-  </si>
-  <si>
-    <t>1 PTA4</t>
-  </si>
-  <si>
-    <t>1 PTA5</t>
-  </si>
-  <si>
-    <t>1 PTA12</t>
-  </si>
-  <si>
-    <t>Odd pins on top -  higher numbers are farther to the right when looking at the back</t>
+    <t>J2 11</t>
+  </si>
+  <si>
+    <t>J2 13</t>
+  </si>
+  <si>
+    <t>J2 19</t>
+  </si>
+  <si>
+    <t>PTC8</t>
+  </si>
+  <si>
+    <t>PTC9</t>
+  </si>
+  <si>
+    <t>PTC11</t>
+  </si>
+  <si>
+    <t>PTC10</t>
+  </si>
+  <si>
+    <t>PTA13</t>
+  </si>
+  <si>
+    <t>PTD4</t>
+  </si>
+  <si>
+    <t>PTC16</t>
+  </si>
+  <si>
+    <t>PTA12</t>
+  </si>
+  <si>
+    <t>PTA16</t>
+  </si>
+  <si>
+    <t>PTA4</t>
+  </si>
+  <si>
+    <t>PTA17</t>
+  </si>
+  <si>
+    <t>PTA5</t>
+  </si>
+  <si>
+    <t>PTE31</t>
+  </si>
+  <si>
+    <t>PTD7</t>
   </si>
 </sst>
 </file>
@@ -518,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,34 +750,28 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>36</v>
+      <c r="B13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
+      <c r="D14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -691,98 +779,104 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>8</v>
       </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>25</v>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,68 +884,307 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>8</v>
       </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>